<commit_message>
Updated RTM excel table
</commit_message>
<xml_diff>
--- a/KinserRTM1.xlsx
+++ b/KinserRTM1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\auggi\OneDrive\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{766EBF08-1C7E-421E-A1CE-AA9A139D706D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774EC505-0120-4247-B944-63F9065FA9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39094C25-B9F2-4A83-BD3C-82FE222E4D5A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>Req ID</t>
   </si>
@@ -57,16 +57,121 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>The Solution must support missiles launched by the user</t>
+  </si>
+  <si>
+    <t>The Solution must support Ships launched by the solution</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>Mandatory</t>
+  </si>
+  <si>
+    <t>The Solution must end the game when hit count reaches ten</t>
+  </si>
+  <si>
+    <t>The Solution must end the game when user clicks left mouse button</t>
+  </si>
+  <si>
+    <t>The Solution must end the game when user clicks esc key</t>
+  </si>
+  <si>
+    <t>The Solution must end the game if user hasn't launched a missile in last 5 minutes</t>
+  </si>
+  <si>
+    <t>Gameplay</t>
+  </si>
+  <si>
+    <t>End game</t>
+  </si>
+  <si>
+    <t>1.a</t>
+  </si>
+  <si>
+    <t>1.b</t>
+  </si>
+  <si>
+    <t>1.c</t>
+  </si>
+  <si>
+    <t>1.d</t>
+  </si>
+  <si>
+    <t>1.e</t>
+  </si>
+  <si>
+    <t>1.f</t>
+  </si>
+  <si>
+    <t>1.g</t>
+  </si>
+  <si>
+    <t>1.h</t>
+  </si>
+  <si>
+    <t>1.i</t>
+  </si>
+  <si>
+    <t>1.j</t>
+  </si>
+  <si>
+    <t>1.k</t>
+  </si>
+  <si>
+    <t>2.a</t>
+  </si>
+  <si>
+    <t>2.b</t>
+  </si>
+  <si>
+    <t>2.c</t>
+  </si>
+  <si>
+    <t>2.d</t>
+  </si>
+  <si>
+    <t>2.d.i</t>
+  </si>
+  <si>
+    <t>2.d.ii</t>
+  </si>
+  <si>
+    <t>2.d.iii</t>
+  </si>
+  <si>
+    <t>2.d.iii.1</t>
+  </si>
+  <si>
+    <t>2.d.iii.2</t>
+  </si>
+  <si>
+    <t>2.d.iii.3</t>
+  </si>
+  <si>
+    <t>2.d.iii.4</t>
+  </si>
+  <si>
+    <t>Diagram 1, main loop detects key stroke, Diagram 2 draws and spawns missiles.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,8 +197,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,16 +550,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F8DD6D5-42F3-4610-81DD-15C5DF935CB0}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.109375" customWidth="1"/>
-    <col min="2" max="2" width="65.33203125" customWidth="1"/>
+    <col min="2" max="2" width="71.77734375" customWidth="1"/>
     <col min="3" max="5" width="10.109375" customWidth="1"/>
     <col min="6" max="6" width="36.77734375" customWidth="1"/>
     <col min="7" max="7" width="10.109375" customWidth="1"/>
@@ -482,10 +588,227 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>